<commit_message>
Making Integration Tests Work
</commit_message>
<xml_diff>
--- a/Extractor/extractor/input/samplesheet.xlsx
+++ b/Extractor/extractor/input/samplesheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\itwinConnectorSamplegitHub\COBie-extractor\extractor\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\itwinConnectorSamplegitHub\Extractor\extractor\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B07C444-CB14-4888-B7B2-CB2D96E6E0ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B416DB9-54E9-4C1A-94F2-E74006642853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -105,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2933" uniqueCount="803">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2937" uniqueCount="804">
   <si>
     <t>Title</t>
   </si>
@@ -2514,6 +2514,9 @@
   </si>
   <si>
     <t>Units_for_quantity_orquantities_being_observed</t>
+  </si>
+  <si>
+    <t>Device 6</t>
   </si>
 </sst>
 </file>
@@ -14687,10 +14690,10 @@
   <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1"/>
+      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14862,12 +14865,30 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="114"/>
-      <c r="C7" s="115"/>
-      <c r="D7" s="127"/>
-      <c r="E7" s="127"/>
-      <c r="F7" s="116"/>
-      <c r="H7" s="125"/>
+      <c r="A7" s="109" t="s">
+        <v>803</v>
+      </c>
+      <c r="B7" s="110">
+        <v>6</v>
+      </c>
+      <c r="C7" s="111">
+        <v>1</v>
+      </c>
+      <c r="D7" s="126">
+        <v>2</v>
+      </c>
+      <c r="E7" s="126">
+        <v>1</v>
+      </c>
+      <c r="F7" s="112" t="s">
+        <v>790</v>
+      </c>
+      <c r="G7" s="109" t="s">
+        <v>786</v>
+      </c>
+      <c r="H7" s="125" t="s">
+        <v>788</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="114"/>

</xml_diff>

<commit_message>
Renamed testProjectId in .env file to projectId
</commit_message>
<xml_diff>
--- a/Extractor/extractor/input/samplesheet.xlsx
+++ b/Extractor/extractor/input/samplesheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\iot\source-code\Rahul\itwinConnectorsample\Extractor\extractor\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\iot\source-code\itwinConnectorsample\Extractor\extractor\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492B09ED-76FC-4BED-BBB2-878A6E743578}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78D2E556-D8A8-42BC-BB4F-21230F412902}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,15 +92,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="21">
   <si>
     <t>Device 1</t>
   </si>
   <si>
     <t>Device 2</t>
-  </si>
-  <si>
-    <t>Device 3</t>
   </si>
   <si>
     <t>Device 4</t>
@@ -122,9 +119,6 @@
   </si>
   <si>
     <t>0x1b</t>
-  </si>
-  <si>
-    <t>0x1c</t>
   </si>
   <si>
     <t>0x2a</t>
@@ -158,6 +152,9 @@
   </si>
   <si>
     <t>Device 5</t>
+  </si>
+  <si>
+    <t>Device 7</t>
   </si>
 </sst>
 </file>
@@ -1197,7 +1194,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1213,28 +1210,28 @@
   <sheetData>
     <row r="1" spans="1:9" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>16</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>18</v>
       </c>
       <c r="I1" s="18"/>
     </row>
@@ -1255,13 +1252,13 @@
         <v>1</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H2" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1281,13 +1278,13 @@
         <v>2</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H3" s="19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1295,30 +1292,30 @@
         <v>2</v>
       </c>
       <c r="B4" s="4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="5">
+        <v>10</v>
+      </c>
+      <c r="D4" s="20">
+        <v>2</v>
+      </c>
+      <c r="E4" s="20">
+        <v>4</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="5">
+      <c r="H4" s="19" t="s">
         <v>5</v>
-      </c>
-      <c r="D4" s="20">
-        <v>7</v>
-      </c>
-      <c r="E4" s="20">
-        <v>3</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H4" s="19" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4">
         <v>4</v>
@@ -1330,21 +1327,21 @@
         <v>2</v>
       </c>
       <c r="E5" s="20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5" s="19" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" s="4">
         <v>4</v>
@@ -1356,21 +1353,21 @@
         <v>2</v>
       </c>
       <c r="E6" s="20">
+        <v>6</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="19" t="s">
         <v>5</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="19" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B7" s="4">
         <v>4</v>
@@ -1382,16 +1379,16 @@
         <v>2</v>
       </c>
       <c r="E7" s="20">
+        <v>7</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="19" t="s">
         <v>5</v>
-      </c>
-      <c r="H7" s="19" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Refactored some console logs
</commit_message>
<xml_diff>
--- a/Extractor/extractor/input/samplesheet.xlsx
+++ b/Extractor/extractor/input/samplesheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\itwinConnectorSamplegitHub\Extractor\extractor\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\iot\source-code\itwinConnectorsample\Extractor\extractor\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F520C3E4-9F83-4AD2-87CD-43CAD3DBA11F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E1A37F7-2EF2-480B-AC3E-3427181C5E08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Device" sheetId="16" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Device!$A$1:$G$4965</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Device!$A$1:$G$4961</definedName>
     <definedName name="ApprovalBy">#REF!</definedName>
     <definedName name="AreaUnit">#REF!</definedName>
     <definedName name="Assembly.Name">#REF!</definedName>
@@ -145,13 +145,13 @@
     <t>Deviceid</t>
   </si>
   <si>
-    <t>Device 7-m</t>
+    <t>Device 5</t>
   </si>
   <si>
-    <t>Device 5-renamed8</t>
+    <t>Device 3</t>
   </si>
   <si>
-    <t>Device 8-m</t>
+    <t>Device 4</t>
   </si>
 </sst>
 </file>
@@ -1181,13 +1181,13 @@
   <sheetPr codeName="Sheet16">
     <tabColor indexed="42"/>
   </sheetPr>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1281,31 +1281,63 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="18"/>
+      <c r="A4" s="3">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="4">
+        <v>10</v>
+      </c>
+      <c r="D4" s="19">
+        <v>2</v>
+      </c>
+      <c r="E4" s="19">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="18" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="19"/>
-      <c r="E5" s="19"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="18"/>
+      <c r="A5" s="3">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="4">
+        <v>10</v>
+      </c>
+      <c r="D5" s="19">
+        <v>2</v>
+      </c>
+      <c r="E5" s="19">
+        <v>7</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="4">
         <v>10</v>
@@ -1314,69 +1346,41 @@
         <v>2</v>
       </c>
       <c r="E6" s="19">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5" t="s">
         <v>8</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H6" s="18" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="7" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="18"/>
+    </row>
     <row r="8" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" s="4">
-        <v>10</v>
-      </c>
-      <c r="D8" s="19">
-        <v>2</v>
-      </c>
-      <c r="E8" s="19">
-        <v>7</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="9"/>
     </row>
     <row r="9" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" s="4">
-        <v>10</v>
-      </c>
-      <c r="D9" s="19">
-        <v>2</v>
-      </c>
-      <c r="E9" s="19">
-        <v>7</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>4</v>
-      </c>
+      <c r="B9" s="7"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="9"/>
     </row>
     <row r="10" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="7"/>
@@ -1588,33 +1592,41 @@
       <c r="E39" s="20"/>
       <c r="F39" s="9"/>
     </row>
-    <row r="40" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B40" s="7"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
+    <row r="40" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="10"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+      <c r="E40" s="12"/>
       <c r="F40" s="9"/>
-    </row>
-    <row r="41" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="7"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="10"/>
+      <c r="B41" s="11"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+      <c r="E41" s="12"/>
       <c r="F41" s="9"/>
-    </row>
-    <row r="42" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="7"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="10"/>
+      <c r="B42" s="11"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+      <c r="E42" s="12"/>
       <c r="F42" s="9"/>
-    </row>
-    <row r="43" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B43" s="7"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="10"/>
+      <c r="B43" s="11"/>
+      <c r="C43" s="12"/>
+      <c r="D43" s="12"/>
+      <c r="E43" s="12"/>
       <c r="F43" s="9"/>
+      <c r="G43" s="10"/>
     </row>
     <row r="44" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="10"/>
@@ -1689,58 +1701,58 @@
       <c r="G51" s="10"/>
     </row>
     <row r="52" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
+      <c r="A52" s="14"/>
       <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="12"/>
-      <c r="E52" s="12"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="20"/>
+      <c r="E52" s="20"/>
       <c r="F52" s="9"/>
-      <c r="G52" s="10"/>
+      <c r="G52" s="14"/>
     </row>
     <row r="53" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
+      <c r="A53" s="14"/>
       <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
-      <c r="D53" s="12"/>
-      <c r="E53" s="12"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="20"/>
+      <c r="E53" s="20"/>
       <c r="F53" s="9"/>
-      <c r="G53" s="10"/>
+      <c r="G53" s="14"/>
     </row>
     <row r="54" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="10"/>
+      <c r="A54" s="14"/>
       <c r="B54" s="11"/>
-      <c r="C54" s="12"/>
-      <c r="D54" s="12"/>
-      <c r="E54" s="12"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="20"/>
+      <c r="E54" s="20"/>
       <c r="F54" s="9"/>
-      <c r="G54" s="10"/>
+      <c r="G54" s="14"/>
     </row>
     <row r="55" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="10"/>
+      <c r="A55" s="14"/>
       <c r="B55" s="11"/>
-      <c r="C55" s="12"/>
-      <c r="D55" s="12"/>
-      <c r="E55" s="12"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="20"/>
       <c r="F55" s="9"/>
-      <c r="G55" s="10"/>
+      <c r="G55" s="14"/>
     </row>
     <row r="56" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="14"/>
+      <c r="A56" s="15"/>
       <c r="B56" s="11"/>
       <c r="C56" s="8"/>
       <c r="D56" s="20"/>
       <c r="E56" s="20"/>
       <c r="F56" s="9"/>
-      <c r="G56" s="14"/>
+      <c r="G56" s="15"/>
     </row>
     <row r="57" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="14"/>
+      <c r="A57" s="15"/>
       <c r="B57" s="11"/>
       <c r="C57" s="8"/>
       <c r="D57" s="20"/>
       <c r="E57" s="20"/>
       <c r="F57" s="9"/>
-      <c r="G57" s="14"/>
+      <c r="G57" s="15"/>
     </row>
     <row r="58" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="14"/>
@@ -1761,22 +1773,22 @@
       <c r="G59" s="14"/>
     </row>
     <row r="60" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="15"/>
+      <c r="A60" s="14"/>
       <c r="B60" s="11"/>
       <c r="C60" s="8"/>
       <c r="D60" s="20"/>
       <c r="E60" s="20"/>
       <c r="F60" s="9"/>
-      <c r="G60" s="15"/>
+      <c r="G60" s="14"/>
     </row>
     <row r="61" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="15"/>
+      <c r="A61" s="14"/>
       <c r="B61" s="11"/>
       <c r="C61" s="8"/>
       <c r="D61" s="20"/>
       <c r="E61" s="20"/>
       <c r="F61" s="9"/>
-      <c r="G61" s="15"/>
+      <c r="G61" s="14"/>
     </row>
     <row r="62" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="14"/>
@@ -1807,7 +1819,7 @@
     </row>
     <row r="65" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A65" s="14"/>
-      <c r="B65" s="11"/>
+      <c r="B65" s="10"/>
       <c r="C65" s="8"/>
       <c r="D65" s="20"/>
       <c r="E65" s="20"/>
@@ -1816,7 +1828,7 @@
     </row>
     <row r="66" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A66" s="14"/>
-      <c r="B66" s="11"/>
+      <c r="B66" s="10"/>
       <c r="C66" s="8"/>
       <c r="D66" s="20"/>
       <c r="E66" s="20"/>
@@ -1825,7 +1837,7 @@
     </row>
     <row r="67" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="14"/>
-      <c r="B67" s="11"/>
+      <c r="B67" s="10"/>
       <c r="C67" s="8"/>
       <c r="D67" s="20"/>
       <c r="E67" s="20"/>
@@ -1834,7 +1846,7 @@
     </row>
     <row r="68" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="14"/>
-      <c r="B68" s="11"/>
+      <c r="B68" s="10"/>
       <c r="C68" s="8"/>
       <c r="D68" s="20"/>
       <c r="E68" s="20"/>
@@ -1941,31 +1953,31 @@
       <c r="G79" s="14"/>
     </row>
     <row r="80" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="14"/>
+      <c r="A80" s="16"/>
       <c r="B80" s="10"/>
       <c r="C80" s="8"/>
       <c r="D80" s="20"/>
       <c r="E80" s="20"/>
       <c r="F80" s="9"/>
-      <c r="G80" s="14"/>
+      <c r="G80" s="16"/>
     </row>
     <row r="81" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="14"/>
+      <c r="A81" s="16"/>
       <c r="B81" s="10"/>
       <c r="C81" s="8"/>
       <c r="D81" s="20"/>
       <c r="E81" s="20"/>
       <c r="F81" s="9"/>
-      <c r="G81" s="14"/>
+      <c r="G81" s="16"/>
     </row>
     <row r="82" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="14"/>
+      <c r="A82" s="16"/>
       <c r="B82" s="10"/>
       <c r="C82" s="8"/>
       <c r="D82" s="20"/>
       <c r="E82" s="20"/>
       <c r="F82" s="9"/>
-      <c r="G82" s="14"/>
+      <c r="G82" s="16"/>
     </row>
     <row r="83" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="14"/>
@@ -1977,31 +1989,31 @@
       <c r="G83" s="14"/>
     </row>
     <row r="84" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A84" s="16"/>
+      <c r="A84" s="14"/>
       <c r="B84" s="10"/>
       <c r="C84" s="8"/>
       <c r="D84" s="20"/>
       <c r="E84" s="20"/>
       <c r="F84" s="9"/>
-      <c r="G84" s="16"/>
+      <c r="G84" s="14"/>
     </row>
     <row r="85" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="16"/>
+      <c r="A85" s="14"/>
       <c r="B85" s="10"/>
       <c r="C85" s="8"/>
       <c r="D85" s="20"/>
       <c r="E85" s="20"/>
       <c r="F85" s="9"/>
-      <c r="G85" s="16"/>
+      <c r="G85" s="14"/>
     </row>
     <row r="86" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="16"/>
+      <c r="A86" s="14"/>
       <c r="B86" s="10"/>
       <c r="C86" s="8"/>
       <c r="D86" s="20"/>
       <c r="E86" s="20"/>
       <c r="F86" s="9"/>
-      <c r="G86" s="16"/>
+      <c r="G86" s="14"/>
     </row>
     <row r="87" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="14"/>
@@ -2048,44 +2060,8 @@
       <c r="F91" s="9"/>
       <c r="G91" s="14"/>
     </row>
-    <row r="92" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="14"/>
-      <c r="B92" s="10"/>
-      <c r="C92" s="8"/>
-      <c r="D92" s="20"/>
-      <c r="E92" s="20"/>
-      <c r="F92" s="9"/>
-      <c r="G92" s="14"/>
-    </row>
-    <row r="93" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="14"/>
-      <c r="B93" s="10"/>
-      <c r="C93" s="8"/>
-      <c r="D93" s="20"/>
-      <c r="E93" s="20"/>
-      <c r="F93" s="9"/>
-      <c r="G93" s="14"/>
-    </row>
-    <row r="94" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A94" s="14"/>
-      <c r="B94" s="10"/>
-      <c r="C94" s="8"/>
-      <c r="D94" s="20"/>
-      <c r="E94" s="20"/>
-      <c r="F94" s="9"/>
-      <c r="G94" s="14"/>
-    </row>
-    <row r="95" spans="1:7" s="13" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="14"/>
-      <c r="B95" s="10"/>
-      <c r="C95" s="8"/>
-      <c r="D95" s="20"/>
-      <c r="E95" s="20"/>
-      <c r="F95" s="9"/>
-      <c r="G95" s="14"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G95" xr:uid="{00000000-0009-0000-0000-00000F000000}"/>
+  <autoFilter ref="A1:G91" xr:uid="{00000000-0009-0000-0000-00000F000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fix for insert element error for iot:device class element
</commit_message>
<xml_diff>
--- a/Extractor/extractor/input/samplesheet.xlsx
+++ b/Extractor/extractor/input/samplesheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\iot\source-code\itwinConnectorsample\Extractor\extractor\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D614FE95-4E52-4557-ACA7-C6EB7E9C7EDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3A30E7-7439-4281-8F5B-3C970703E934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -92,7 +92,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
   <si>
     <t>Device 1</t>
   </si>
@@ -103,16 +103,19 @@
     <t>Celsius</t>
   </si>
   <si>
-    <t>DeviceType</t>
+    <t>units_for_quantities_being_observed</t>
   </si>
   <si>
-    <t>Units_for_quantity_orquantities_being_observed</t>
+    <t>type_of_quantity_observed</t>
   </si>
   <si>
-    <t>Type_of_quantity_observed</t>
+    <t>devicetype</t>
   </si>
   <si>
-    <t>Deviceid</t>
+    <t>deviceid</t>
+  </si>
+  <si>
+    <t>Device 2</t>
   </si>
 </sst>
 </file>
@@ -1135,7 +1138,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:XFD6"/>
+      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1152,13 +1155,13 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E1" s="12"/>
     </row>
@@ -1177,10 +1180,18 @@
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="13"/>
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>

</xml_diff>

<commit_message>
Added datapoint and other schema classes
</commit_message>
<xml_diff>
--- a/Extractor/extractor/input/samplesheet.xlsx
+++ b/Extractor/extractor/input/samplesheet.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\iot\source-code\itwinConnectorsample\Extractor\extractor\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC3A30E7-7439-4281-8F5B-3C970703E934}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C93D08E-9324-4FDE-820B-0543D8B07F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="16" r:id="rId1"/>
+    <sheet name="TemperatureDatapoint" sheetId="17" r:id="rId2"/>
+    <sheet name="PressureDatapoint" sheetId="18" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Device!$A$1:$C$4961</definedName>
@@ -92,30 +94,78 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
-  <si>
-    <t>Device 1</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+  <si>
+    <t>Celsius</t>
+  </si>
+  <si>
+    <t>units_for_quantities_being_observed</t>
+  </si>
+  <si>
+    <t>type_of_quantity_observed</t>
+  </si>
+  <si>
+    <t>devicetype</t>
+  </si>
+  <si>
+    <t>deviceid</t>
+  </si>
+  <si>
+    <t>Device 11</t>
+  </si>
+  <si>
+    <t>Temperature 123</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>unit</t>
+  </si>
+  <si>
+    <t>T-1</t>
+  </si>
+  <si>
+    <t>T-2</t>
+  </si>
+  <si>
+    <t>P-1</t>
+  </si>
+  <si>
+    <t>P-2</t>
+  </si>
+  <si>
+    <t>unit 1 for P-1</t>
+  </si>
+  <si>
+    <t>unit 2 for P-2</t>
+  </si>
+  <si>
+    <t>unit 1 for T-1</t>
+  </si>
+  <si>
+    <t>unit 2 for T-2</t>
   </si>
   <si>
     <t xml:space="preserve">Temperature </t>
   </si>
   <si>
-    <t>Celsius</t>
-  </si>
-  <si>
-    <t>units_for_quantities_being_observed</t>
-  </si>
-  <si>
-    <t>type_of_quantity_observed</t>
-  </si>
-  <si>
-    <t>devicetype</t>
-  </si>
-  <si>
-    <t>deviceid</t>
-  </si>
-  <si>
-    <t>Device 2</t>
+    <t>Device 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pressure </t>
+  </si>
+  <si>
+    <t>mm hg</t>
+  </si>
+  <si>
+    <t>Device 5</t>
+  </si>
+  <si>
+    <t>Device 6</t>
+  </si>
+  <si>
+    <t>Device 7</t>
   </si>
 </sst>
 </file>
@@ -1134,11 +1184,11 @@
   </sheetPr>
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B3" sqref="B3"/>
+      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1152,16 +1202,16 @@
   <sheetData>
     <row r="1" spans="1:5" ht="72.599999999999994" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E1" s="12"/>
     </row>
@@ -1170,46 +1220,70 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>0</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="13" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3">
+        <v>4</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3">
         <v>7</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="13"/>
-    </row>
-    <row r="5" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="13"/>
-    </row>
-    <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="13"/>
+      <c r="B6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -1578,4 +1652,128 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8DE4B46-B99D-4DA6-A19C-4FF67C7C96BE}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="29.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4150DC4B-4AA6-4F20-9B7E-B84A6D08CA45}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="20.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C3">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed issue for name and unit values not appearing in iModel
</commit_message>
<xml_diff>
--- a/Extractor/extractor/input/samplesheet.xlsx
+++ b/Extractor/extractor/input/samplesheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\iot\source-code\itwinConnectorsample\Extractor\extractor\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C93D08E-9324-4FDE-820B-0543D8B07F10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76669055-2BED-4480-A91A-8A550833A50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="16" r:id="rId1"/>
@@ -165,7 +165,7 @@
     <t>Device 6</t>
   </si>
   <si>
-    <t>Device 7</t>
+    <t>Device 8</t>
   </si>
 </sst>
 </file>
@@ -1184,11 +1184,11 @@
   </sheetPr>
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1273,16 +1273,16 @@
     </row>
     <row r="6" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>20</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -1659,7 +1659,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1731,8 +1731,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4150DC4B-4AA6-4F20-9B7E-B84A6D08CA45}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1759,7 +1759,7 @@
         <v>13</v>
       </c>
       <c r="C2">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1770,7 +1770,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implementation for relationship classes
</commit_message>
<xml_diff>
--- a/Extractor/extractor/input/samplesheet.xlsx
+++ b/Extractor/extractor/input/samplesheet.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\iot\source-code\itwinConnectorsample\Extractor\extractor\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76669055-2BED-4480-A91A-8A550833A50D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC4DFA44-C8A1-4857-8F6F-1D60E1912EA8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="804" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="16" r:id="rId1"/>
     <sheet name="TemperatureDatapoint" sheetId="17" r:id="rId2"/>
     <sheet name="PressureDatapoint" sheetId="18" r:id="rId3"/>
+    <sheet name="DatapointObservesSpatialElement" sheetId="19" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Device!$A$1:$C$4961</definedName>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Celsius</t>
   </si>
@@ -1184,7 +1185,7 @@
   </sheetPr>
   <dimension ref="A1:E91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1659,7 +1660,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1776,4 +1777,44 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{265C5DD8-1F90-4BAE-89FD-673E563BBAE9}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>